<commit_message>
add more input files
</commit_message>
<xml_diff>
--- a/output/csc_version_indicator_poverty_aggregates.xlsx
+++ b/output/csc_version_indicator_poverty_aggregates.xlsx
@@ -1,19 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/acastanedaa_worldbank_org/Documents/WorldBank/DECDG/PovcalNet Team/OPCS-data-submission/output/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_305B0EA7883F23BEA55FC707F0012D16618CA6C2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7ADD9F71-A853-4809-822E-1BB4B1828C7D}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" fullCalcOnLoad="true"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="168" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="87">
   <si>
     <t>Region</t>
   </si>
@@ -279,7 +286,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -302,30 +309,346 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BN35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:66">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -525,7 +848,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:66">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -599,7 +922,7 @@
       <c r="BM2" s="1"/>
       <c r="BN2" s="1"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:66">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -673,7 +996,7 @@
       <c r="BM3" s="1"/>
       <c r="BN3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:66">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -747,7 +1070,7 @@
       <c r="BM4" s="1"/>
       <c r="BN4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:66">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -821,7 +1144,7 @@
       <c r="BM5" s="1"/>
       <c r="BN5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:66">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -895,7 +1218,7 @@
       <c r="BM6" s="1"/>
       <c r="BN6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:66">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -969,7 +1292,7 @@
       <c r="BM7" s="1"/>
       <c r="BN7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:66">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1043,7 +1366,7 @@
       <c r="BM8" s="1"/>
       <c r="BN8" s="1"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:66">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1117,7 +1440,7 @@
       <c r="BM9" s="1"/>
       <c r="BN9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:66">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1241,7 +1564,7 @@
       <c r="BM10" s="1"/>
       <c r="BN10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:66">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1288,13 +1611,13 @@
         <v>85.2</v>
       </c>
       <c r="AL11" s="1">
-        <v>86.09999999999999</v>
+        <v>86.1</v>
       </c>
       <c r="AM11" s="1">
-        <v>86.09999999999999</v>
+        <v>86.1</v>
       </c>
       <c r="AN11" s="1">
-        <v>86.59999999999999</v>
+        <v>86.6</v>
       </c>
       <c r="AO11" s="1">
         <v>85.8</v>
@@ -1303,7 +1626,7 @@
         <v>84.7</v>
       </c>
       <c r="AQ11" s="1">
-        <v>86.59999999999999</v>
+        <v>86.6</v>
       </c>
       <c r="AR11" s="1"/>
       <c r="AS11" s="1">
@@ -1319,7 +1642,7 @@
         <v>83.2</v>
       </c>
       <c r="AW11" s="1">
-        <v>81.40000000000001</v>
+        <v>81.400000000000006</v>
       </c>
       <c r="AX11" s="1">
         <v>80.7</v>
@@ -1331,10 +1654,10 @@
         <v>79.2</v>
       </c>
       <c r="BA11" s="1">
-        <v>79.40000000000001</v>
+        <v>79.400000000000006</v>
       </c>
       <c r="BB11" s="1">
-        <v>78.59999999999999</v>
+        <v>78.599999999999994</v>
       </c>
       <c r="BC11" s="1">
         <v>78.2</v>
@@ -1349,7 +1672,7 @@
         <v>78</v>
       </c>
       <c r="BG11" s="1">
-        <v>80.40000000000001</v>
+        <v>80.400000000000006</v>
       </c>
       <c r="BH11" s="1">
         <v>80.2</v>
@@ -1365,7 +1688,7 @@
       <c r="BM11" s="1"/>
       <c r="BN11" s="1"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:66">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1517,7 +1840,7 @@
       <c r="BM12" s="1"/>
       <c r="BN12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:66">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1559,7 +1882,7 @@
         <v>5.3</v>
       </c>
       <c r="AC13" s="1">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="AD13" s="1">
         <v>4.7</v>
@@ -1580,7 +1903,7 @@
         <v>3.7</v>
       </c>
       <c r="AJ13" s="1">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AK13" s="1">
         <v>6</v>
@@ -1589,25 +1912,25 @@
         <v>7</v>
       </c>
       <c r="AM13" s="1">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="AN13" s="1">
         <v>6.3</v>
       </c>
       <c r="AO13" s="1">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="AP13" s="1">
         <v>4.3</v>
       </c>
       <c r="AQ13" s="1">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="AR13" s="1">
         <v>4.8</v>
       </c>
       <c r="AS13" s="1">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AT13" s="1">
         <v>4.5</v>
@@ -1652,7 +1975,7 @@
         <v>2.6</v>
       </c>
       <c r="BH13" s="1">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="BI13" s="1">
         <v>2</v>
@@ -1669,7 +1992,7 @@
       <c r="BM13" s="1"/>
       <c r="BN13" s="1"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:66">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1743,7 +2066,7 @@
       <c r="BM14" s="1"/>
       <c r="BN14" s="1"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:66">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1817,7 +2140,7 @@
       <c r="BM15" s="1"/>
       <c r="BN15" s="1"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:66">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1869,13 +2192,13 @@
         <v>93.3</v>
       </c>
       <c r="AK16" s="1">
-        <v>93.59999999999999</v>
+        <v>93.6</v>
       </c>
       <c r="AL16" s="1">
         <v>93.5</v>
       </c>
       <c r="AM16" s="1">
-        <v>93.09999999999999</v>
+        <v>93.1</v>
       </c>
       <c r="AN16" s="1">
         <v>92.8</v>
@@ -1884,10 +2207,10 @@
         <v>92.7</v>
       </c>
       <c r="AP16" s="1">
-        <v>92.40000000000001</v>
+        <v>92.4</v>
       </c>
       <c r="AQ16" s="1">
-        <v>92.59999999999999</v>
+        <v>92.6</v>
       </c>
       <c r="AR16" s="1">
         <v>92.8</v>
@@ -1899,7 +2222,7 @@
         <v>92.7</v>
       </c>
       <c r="AU16" s="1">
-        <v>92.40000000000001</v>
+        <v>92.4</v>
       </c>
       <c r="AV16" s="1">
         <v>91.7</v>
@@ -1914,7 +2237,7 @@
         <v>90.2</v>
       </c>
       <c r="AZ16" s="1">
-        <v>89.59999999999999</v>
+        <v>89.6</v>
       </c>
       <c r="BA16" s="1">
         <v>89.3</v>
@@ -1923,16 +2246,16 @@
         <v>88.7</v>
       </c>
       <c r="BC16" s="1">
-        <v>88.09999999999999</v>
+        <v>88.1</v>
       </c>
       <c r="BD16" s="1">
-        <v>87.90000000000001</v>
+        <v>87.9</v>
       </c>
       <c r="BE16" s="1">
         <v>87.5</v>
       </c>
       <c r="BF16" s="1">
-        <v>86.90000000000001</v>
+        <v>86.9</v>
       </c>
       <c r="BG16" s="1">
         <v>86.8</v>
@@ -1944,16 +2267,16 @@
         <v>86</v>
       </c>
       <c r="BJ16" s="1">
-        <v>85.59999999999999</v>
+        <v>85.6</v>
       </c>
       <c r="BK16" s="1">
-        <v>85.40000000000001</v>
+        <v>85.4</v>
       </c>
       <c r="BL16" s="1"/>
       <c r="BM16" s="1"/>
       <c r="BN16" s="1"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:66">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -2044,7 +2367,7 @@
         <v>40.5</v>
       </c>
       <c r="AX17" s="1">
-        <v>38.8</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="AY17" s="1">
         <v>37</v>
@@ -2089,7 +2412,7 @@
       <c r="BM17" s="1"/>
       <c r="BN17" s="1"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:66">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -2163,7 +2486,7 @@
       <c r="BM18" s="1"/>
       <c r="BN18" s="1"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:66">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -2237,7 +2560,7 @@
       <c r="BM19" s="1"/>
       <c r="BN19" s="1"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:66">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -2311,7 +2634,7 @@
       <c r="BM20" s="1"/>
       <c r="BN20" s="1"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:66">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -2385,7 +2708,7 @@
       <c r="BM21" s="1"/>
       <c r="BN21" s="1"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:66">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -2431,25 +2754,25 @@
       <c r="AK22" s="1"/>
       <c r="AL22" s="1"/>
       <c r="AM22" s="1">
-        <v>93.90000000000001</v>
+        <v>93.9</v>
       </c>
       <c r="AN22" s="1">
         <v>93.7</v>
       </c>
       <c r="AO22" s="1">
-        <v>93.40000000000001</v>
+        <v>93.4</v>
       </c>
       <c r="AP22" s="1">
-        <v>93.09999999999999</v>
+        <v>93.1</v>
       </c>
       <c r="AQ22" s="1">
-        <v>93.40000000000001</v>
+        <v>93.4</v>
       </c>
       <c r="AR22" s="1">
-        <v>93.40000000000001</v>
+        <v>93.4</v>
       </c>
       <c r="AS22" s="1">
-        <v>93.40000000000001</v>
+        <v>93.4</v>
       </c>
       <c r="AT22" s="1">
         <v>93.3</v>
@@ -2470,7 +2793,7 @@
         <v>91.2</v>
       </c>
       <c r="AZ22" s="1">
-        <v>90.40000000000001</v>
+        <v>90.4</v>
       </c>
       <c r="BA22" s="1">
         <v>90.7</v>
@@ -2479,10 +2802,10 @@
         <v>90.3</v>
       </c>
       <c r="BC22" s="1">
-        <v>90.09999999999999</v>
+        <v>90.1</v>
       </c>
       <c r="BD22" s="1">
-        <v>90.90000000000001</v>
+        <v>90.9</v>
       </c>
       <c r="BE22" s="1">
         <v>91.7</v>
@@ -2491,13 +2814,13 @@
         <v>91.7</v>
       </c>
       <c r="BG22" s="1">
-        <v>92.59999999999999</v>
+        <v>92.6</v>
       </c>
       <c r="BH22" s="1">
-        <v>92.40000000000001</v>
+        <v>92.4</v>
       </c>
       <c r="BI22" s="1">
-        <v>92.40000000000001</v>
+        <v>92.4</v>
       </c>
       <c r="BJ22" s="1">
         <v>92.2</v>
@@ -2507,7 +2830,7 @@
       <c r="BM22" s="1"/>
       <c r="BN22" s="1"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:66">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -2629,7 +2952,7 @@
       <c r="BM23" s="1"/>
       <c r="BN23" s="1"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:66">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -2706,7 +3029,7 @@
         <v>40</v>
       </c>
       <c r="AN24" s="1">
-        <v>38.8</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="AO24" s="1"/>
       <c r="AP24" s="1"/>
@@ -2720,7 +3043,7 @@
         <v>35.1</v>
       </c>
       <c r="AV24" s="1">
-        <v>33.3</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="AW24" s="1">
         <v>31.7</v>
@@ -2744,13 +3067,13 @@
         <v>20.5</v>
       </c>
       <c r="BD24" s="1">
-        <v>19.1</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="BE24" s="1">
         <v>18.3</v>
       </c>
       <c r="BF24" s="1">
-        <v>17.4</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="BG24" s="1">
         <v>16.5</v>
@@ -2775,7 +3098,7 @@
       </c>
       <c r="BN24" s="1"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:66">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -2807,16 +3130,16 @@
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="1">
-        <v>90.40000000000001</v>
+        <v>90.4</v>
       </c>
       <c r="Z25" s="1">
-        <v>90.40000000000001</v>
+        <v>90.4</v>
       </c>
       <c r="AA25" s="1">
         <v>90.2</v>
       </c>
       <c r="AB25" s="1">
-        <v>89.90000000000001</v>
+        <v>89.9</v>
       </c>
       <c r="AC25" s="1">
         <v>89.8</v>
@@ -2828,7 +3151,7 @@
         <v>90</v>
       </c>
       <c r="AF25" s="1">
-        <v>89.90000000000001</v>
+        <v>89.9</v>
       </c>
       <c r="AG25" s="1">
         <v>89.8</v>
@@ -2852,7 +3175,7 @@
         <v>90</v>
       </c>
       <c r="AN25" s="1">
-        <v>89.90000000000001</v>
+        <v>89.9</v>
       </c>
       <c r="AO25" s="1"/>
       <c r="AP25" s="1"/>
@@ -2860,16 +3183,16 @@
       <c r="AR25" s="1"/>
       <c r="AS25" s="1"/>
       <c r="AT25" s="1">
-        <v>88.40000000000001</v>
+        <v>88.4</v>
       </c>
       <c r="AU25" s="1">
         <v>88</v>
       </c>
       <c r="AV25" s="1">
-        <v>87.09999999999999</v>
+        <v>87.1</v>
       </c>
       <c r="AW25" s="1">
-        <v>86.40000000000001</v>
+        <v>86.4</v>
       </c>
       <c r="AX25" s="1">
         <v>85.7</v>
@@ -2878,7 +3201,7 @@
         <v>85.2</v>
       </c>
       <c r="AZ25" s="1">
-        <v>84.59999999999999</v>
+        <v>84.6</v>
       </c>
       <c r="BA25" s="1">
         <v>84</v>
@@ -2887,7 +3210,7 @@
         <v>82.3</v>
       </c>
       <c r="BC25" s="1">
-        <v>80.90000000000001</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="BD25" s="1">
         <v>80</v>
@@ -2896,7 +3219,7 @@
         <v>79.3</v>
       </c>
       <c r="BF25" s="1">
-        <v>78.59999999999999</v>
+        <v>78.599999999999994</v>
       </c>
       <c r="BG25" s="1">
         <v>78.2</v>
@@ -2905,7 +3228,7 @@
         <v>77.8</v>
       </c>
       <c r="BI25" s="1">
-        <v>76.40000000000001</v>
+        <v>76.400000000000006</v>
       </c>
       <c r="BJ25" s="1">
         <v>74.8</v>
@@ -2921,7 +3244,7 @@
       </c>
       <c r="BN25" s="1"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:66">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -2995,7 +3318,7 @@
       <c r="BM26" s="1"/>
       <c r="BN26" s="1"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:66">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -3069,7 +3392,7 @@
       <c r="BM27" s="1"/>
       <c r="BN27" s="1"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:66">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -3154,13 +3477,13 @@
       <c r="AR28" s="1"/>
       <c r="AS28" s="1"/>
       <c r="AT28" s="1">
-        <v>39.8</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="AU28" s="1">
         <v>38.6</v>
       </c>
       <c r="AV28" s="1">
-        <v>36.8</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="AW28" s="1">
         <v>34.9</v>
@@ -3184,16 +3507,16 @@
         <v>21.4</v>
       </c>
       <c r="BD28" s="1">
-        <v>19.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="BE28" s="1">
-        <v>18.9</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="BF28" s="1">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="BG28" s="1">
-        <v>16.6</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="BH28" s="1">
         <v>15.8</v>
@@ -3215,7 +3538,7 @@
       </c>
       <c r="BN28" s="1"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:66">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -3253,7 +3576,7 @@
         <v>97.5</v>
       </c>
       <c r="AA29" s="1">
-        <v>97.40000000000001</v>
+        <v>97.4</v>
       </c>
       <c r="AB29" s="1">
         <v>97.2</v>
@@ -3268,31 +3591,31 @@
         <v>96.7</v>
       </c>
       <c r="AF29" s="1">
-        <v>96.59999999999999</v>
+        <v>96.6</v>
       </c>
       <c r="AG29" s="1">
-        <v>96.59999999999999</v>
+        <v>96.6</v>
       </c>
       <c r="AH29" s="1">
-        <v>96.59999999999999</v>
+        <v>96.6</v>
       </c>
       <c r="AI29" s="1">
-        <v>96.59999999999999</v>
+        <v>96.6</v>
       </c>
       <c r="AJ29" s="1">
         <v>96.5</v>
       </c>
       <c r="AK29" s="1">
-        <v>96.40000000000001</v>
+        <v>96.4</v>
       </c>
       <c r="AL29" s="1">
-        <v>96.09999999999999</v>
+        <v>96.1</v>
       </c>
       <c r="AM29" s="1">
         <v>95.8</v>
       </c>
       <c r="AN29" s="1">
-        <v>95.59999999999999</v>
+        <v>95.6</v>
       </c>
       <c r="AO29" s="1"/>
       <c r="AP29" s="1"/>
@@ -3300,7 +3623,7 @@
       <c r="AR29" s="1"/>
       <c r="AS29" s="1"/>
       <c r="AT29" s="1">
-        <v>94.59999999999999</v>
+        <v>94.6</v>
       </c>
       <c r="AU29" s="1">
         <v>94.2</v>
@@ -3315,7 +3638,7 @@
         <v>93</v>
       </c>
       <c r="AY29" s="1">
-        <v>92.59999999999999</v>
+        <v>92.6</v>
       </c>
       <c r="AZ29" s="1">
         <v>92.3</v>
@@ -3336,10 +3659,10 @@
         <v>88.5</v>
       </c>
       <c r="BF29" s="1">
-        <v>88.09999999999999</v>
+        <v>88.1</v>
       </c>
       <c r="BG29" s="1">
-        <v>87.59999999999999</v>
+        <v>87.6</v>
       </c>
       <c r="BH29" s="1">
         <v>87.2</v>
@@ -3361,7 +3684,7 @@
       </c>
       <c r="BN29" s="1"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:66">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -3435,7 +3758,7 @@
       <c r="BM30" s="1"/>
       <c r="BN30" s="1"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:66">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -3509,7 +3832,7 @@
       <c r="BM31" s="1"/>
       <c r="BN31" s="1"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:66">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -3580,16 +3903,16 @@
         <v>43.6</v>
       </c>
       <c r="AL32" s="1">
-        <v>40.2</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="AM32" s="1">
         <v>37.6</v>
       </c>
       <c r="AN32" s="1">
-        <v>34.8</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="AO32" s="1">
-        <v>34.7</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="AP32" s="1">
         <v>35.4</v>
@@ -3610,10 +3933,10 @@
         <v>22.9</v>
       </c>
       <c r="AV32" s="1">
-        <v>20.1</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="AW32" s="1">
-        <v>16.6</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="AX32" s="1">
         <v>16</v>
@@ -3631,7 +3954,7 @@
         <v>10.6</v>
       </c>
       <c r="BC32" s="1">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="BD32" s="1">
         <v>7.1</v>
@@ -3649,7 +3972,7 @@
         <v>2.4</v>
       </c>
       <c r="BI32" s="1">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="BJ32" s="1">
         <v>2</v>
@@ -3663,7 +3986,7 @@
       <c r="BM32" s="1"/>
       <c r="BN32" s="1"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:66">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -3695,16 +4018,16 @@
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
       <c r="Y33" s="1">
-        <v>80.59999999999999</v>
+        <v>80.599999999999994</v>
       </c>
       <c r="Z33" s="1">
-        <v>80.59999999999999</v>
+        <v>80.599999999999994</v>
       </c>
       <c r="AA33" s="1">
         <v>81.2</v>
       </c>
       <c r="AB33" s="1">
-        <v>81.09999999999999</v>
+        <v>81.099999999999994</v>
       </c>
       <c r="AC33" s="1">
         <v>80.8</v>
@@ -3716,7 +4039,7 @@
         <v>79.8</v>
       </c>
       <c r="AF33" s="1">
-        <v>79.90000000000001</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="AG33" s="1">
         <v>79.7</v>
@@ -3725,37 +4048,37 @@
         <v>79.7</v>
       </c>
       <c r="AI33" s="1">
-        <v>80.40000000000001</v>
+        <v>80.400000000000006</v>
       </c>
       <c r="AJ33" s="1">
-        <v>80.90000000000001</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="AK33" s="1">
         <v>80.8</v>
       </c>
       <c r="AL33" s="1">
-        <v>80.09999999999999</v>
+        <v>80.099999999999994</v>
       </c>
       <c r="AM33" s="1">
         <v>79.3</v>
       </c>
       <c r="AN33" s="1">
-        <v>78.59999999999999</v>
+        <v>78.599999999999994</v>
       </c>
       <c r="AO33" s="1">
-        <v>78.09999999999999</v>
+        <v>78.099999999999994</v>
       </c>
       <c r="AP33" s="1">
-        <v>77.90000000000001</v>
+        <v>77.900000000000006</v>
       </c>
       <c r="AQ33" s="1">
-        <v>78.09999999999999</v>
+        <v>78.099999999999994</v>
       </c>
       <c r="AR33" s="1">
-        <v>75.90000000000001</v>
+        <v>75.900000000000006</v>
       </c>
       <c r="AS33" s="1">
-        <v>74.40000000000001</v>
+        <v>74.400000000000006</v>
       </c>
       <c r="AT33" s="1">
         <v>72</v>
@@ -3767,7 +4090,7 @@
         <v>68.2</v>
       </c>
       <c r="AW33" s="1">
-        <v>65.09999999999999</v>
+        <v>65.099999999999994</v>
       </c>
       <c r="AX33" s="1">
         <v>62.4</v>
@@ -3817,7 +4140,7 @@
       <c r="BM33" s="1"/>
       <c r="BN33" s="1"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:66">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -3861,7 +4184,7 @@
         <v>41.1</v>
       </c>
       <c r="AC34" s="1">
-        <v>39.7</v>
+        <v>39.700000000000003</v>
       </c>
       <c r="AD34" s="1">
         <v>38.4</v>
@@ -3870,7 +4193,7 @@
         <v>37.4</v>
       </c>
       <c r="AF34" s="1">
-        <v>35.7</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="AG34" s="1">
         <v>38.4</v>
@@ -3885,7 +4208,7 @@
         <v>36.5</v>
       </c>
       <c r="AK34" s="1">
-        <v>35.7</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="AL34" s="1">
         <v>34.4</v>
@@ -3927,13 +4250,13 @@
         <v>20.9</v>
       </c>
       <c r="AY34" s="1">
-        <v>19.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="AZ34" s="1">
         <v>18.8</v>
       </c>
       <c r="BA34" s="1">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="BB34" s="1">
         <v>16.3</v>
@@ -3957,7 +4280,7 @@
         <v>10.5</v>
       </c>
       <c r="BI34" s="1">
-        <v>9.800000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="BJ34" s="1">
         <v>9.1</v>
@@ -3969,7 +4292,7 @@
       <c r="BM34" s="1"/>
       <c r="BN34" s="1"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:66">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -4010,7 +4333,7 @@
         <v>68.8</v>
       </c>
       <c r="AB35" s="1">
-        <v>68.90000000000001</v>
+        <v>68.900000000000006</v>
       </c>
       <c r="AC35" s="1">
         <v>68.7</v>
@@ -4019,7 +4342,7 @@
         <v>68.3</v>
       </c>
       <c r="AE35" s="1">
-        <v>68.59999999999999</v>
+        <v>68.599999999999994</v>
       </c>
       <c r="AF35" s="1">
         <v>68.7</v>
@@ -4028,13 +4351,13 @@
         <v>68.8</v>
       </c>
       <c r="AH35" s="1">
-        <v>68.90000000000001</v>
+        <v>68.900000000000006</v>
       </c>
       <c r="AI35" s="1">
-        <v>69.40000000000001</v>
+        <v>69.400000000000006</v>
       </c>
       <c r="AJ35" s="1">
-        <v>69.90000000000001</v>
+        <v>69.900000000000006</v>
       </c>
       <c r="AK35" s="1">
         <v>70.5</v>
@@ -4043,7 +4366,7 @@
         <v>70.5</v>
       </c>
       <c r="AM35" s="1">
-        <v>69.90000000000001</v>
+        <v>69.900000000000006</v>
       </c>
       <c r="AN35" s="1">
         <v>70</v>
@@ -4058,22 +4381,22 @@
         <v>69.8</v>
       </c>
       <c r="AR35" s="1">
-        <v>68.90000000000001</v>
+        <v>68.900000000000006</v>
       </c>
       <c r="AS35" s="1">
         <v>68.3</v>
       </c>
       <c r="AT35" s="1">
-        <v>67.40000000000001</v>
+        <v>67.400000000000006</v>
       </c>
       <c r="AU35" s="1">
-        <v>66.90000000000001</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="AV35" s="1">
-        <v>65.59999999999999</v>
+        <v>65.599999999999994</v>
       </c>
       <c r="AW35" s="1">
-        <v>64.09999999999999</v>
+        <v>64.099999999999994</v>
       </c>
       <c r="AX35" s="1">
         <v>62.9</v>
@@ -4122,5 +4445,6 @@
       <c r="BN35" s="1"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>